<commit_message>
improve the wer result
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>features_ground</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t xml:space="preserve">77, 0.5674 </t>
+  </si>
+  <si>
+    <t>features_custom_2</t>
+  </si>
+  <si>
+    <t>76,0.573</t>
+  </si>
+  <si>
+    <t>102,0.4269</t>
+  </si>
+  <si>
+    <t>103,0.4213</t>
+  </si>
+  <si>
+    <t>90,0.4943</t>
   </si>
 </sst>
 </file>
@@ -573,7 +588,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,11 +715,21 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>